<commit_message>
metadata updated - v1.4
</commit_message>
<xml_diff>
--- a/utils/Data Dictionary.xlsx
+++ b/utils/Data Dictionary.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="147">
   <si>
     <t>Description</t>
   </si>
@@ -435,6 +435,36 @@
   <si>
     <t>A binary parameter used for inpainting the extracted frames from the video files</t>
   </si>
+  <si>
+    <t>date_added</t>
+  </si>
+  <si>
+    <t>Files added in the respective version of the dataset</t>
+  </si>
+  <si>
+    <t>case_no</t>
+  </si>
+  <si>
+    <t>paper_link</t>
+  </si>
+  <si>
+    <t>paper_doi</t>
+  </si>
+  <si>
+    <t>license</t>
+  </si>
+  <si>
+    <t>Patient cases</t>
+  </si>
+  <si>
+    <t>Link to the paper for files extracted from scientific publications</t>
+  </si>
+  <si>
+    <t>DOI of the paper for files extracted from scientific publications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">License </t>
+  </si>
 </sst>
 </file>
 
@@ -616,7 +646,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> v1.2.</a:t>
+            <a:t> v1.4.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -669,7 +699,7 @@
               <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
               <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
             </a:rPr>
-            <a:t> April 12, 2021</a:t>
+            <a:t> July 13, 2021</a:t>
           </a:r>
           <a:endParaRPr lang="en-CA" sz="1100" b="0">
             <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
@@ -952,7 +982,7 @@
   </sheetPr>
   <dimension ref="A10:V998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
@@ -24940,10 +24970,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25156,14 +25186,14 @@
         <v>41</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
@@ -25171,19 +25201,17 @@
         <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>52</v>
-      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="4" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
@@ -25191,15 +25219,17 @@
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
       <c r="F13" s="4" t="s">
         <v>53</v>
       </c>
@@ -25209,17 +25239,15 @@
         <v>13</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>56</v>
-      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="4" t="s">
         <v>53</v>
       </c>
@@ -25229,17 +25257,15 @@
         <v>14</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>57</v>
+        <v>143</v>
       </c>
       <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4" t="s">
         <v>53</v>
       </c>
@@ -25249,30 +25275,132 @@
         <v>15</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>56</v>
+      </c>
       <c r="F16" s="4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+    <row r="17" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="4">
+        <v>19</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A21" s="4">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+    </row>
+    <row r="23" spans="1:10" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -25283,8 +25411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25:F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -25775,7 +25903,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>41</v>
+        <v>137</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>50</v>
@@ -25785,8 +25913,50 @@
       </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A26" s="4">
+        <v>25</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="4"/>
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
     </row>
     <row r="30" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B30" s="4"/>
@@ -25849,9 +26019,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -26181,15 +26353,49 @@
         <v>41</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>138</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4" t="s">
-        <v>53</v>
-      </c>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
+    <row r="20" spans="1:6" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>